<commit_message>
fetching all lc data for precise approach
</commit_message>
<xml_diff>
--- a/LCDataDictionary.xlsx
+++ b/LCDataDictionary.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="28615"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23127"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rjoshi/Documents/LendingClub/Quarterly_Loan_Stats/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\huynq1\lending-club-scorecard\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{278A8518-B280-4EFE-ADC8-D53B0C860140}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="22620" activeTab="1"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LoanStats" sheetId="3" r:id="rId1"/>
@@ -17,11 +18,11 @@
     <sheet name="RejectStats" sheetId="7" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">browseNotes!$A$1:$B$89</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">LoanStats!$A$1:$B$129</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">browseNotes!$A$1:$B$121</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">LoanStats!$A$1:$D$152</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">RejectStats!$A$1:$B$10</definedName>
   </definedNames>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="191029" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="568" uniqueCount="383">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="749" uniqueCount="401">
   <si>
     <t>id</t>
   </si>
@@ -1197,11 +1198,65 @@
   <si>
     <t>The method by which the borrower receives their loan. Possible values are: CASH, DIRECT_PAY</t>
   </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t>Ngày gần nhất LC pull lịch sử tín dụng</t>
+  </si>
+  <si>
+    <t>Start observing</t>
+  </si>
+  <si>
+    <t>Sources</t>
+  </si>
+  <si>
+    <t>Demographic</t>
+  </si>
+  <si>
+    <t>Indenture</t>
+  </si>
+  <si>
+    <t>Key</t>
+  </si>
+  <si>
+    <t>publicly available policy_code=1, new products not publicly available policy_code=2</t>
+  </si>
+  <si>
+    <t>Hardship Plan</t>
+  </si>
+  <si>
+    <t>Vay cơ cấu nợ</t>
+  </si>
+  <si>
+    <t>Post Charged-off Behavior</t>
+  </si>
+  <si>
+    <t>Collection Behavior</t>
+  </si>
+  <si>
+    <t>y</t>
+  </si>
+  <si>
+    <t>Self-reported</t>
+  </si>
+  <si>
+    <t>History Behavior</t>
+  </si>
+  <si>
+    <t>Score</t>
+  </si>
+  <si>
+    <t>For family members</t>
+  </si>
+  <si>
+    <t>Secondary Applicants</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="24" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -2250,1346 +2305,2018 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr enableFormatConditionsCalculation="0">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:K154"/>
+  <dimension ref="A1:M154"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A113" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A145" sqref="A145:B145"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="34" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="196.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="118.83203125" style="6" customWidth="1"/>
-    <col min="9" max="9" width="25" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="40.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="27.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="25.28515625" customWidth="1"/>
+    <col min="4" max="4" width="196.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="118.85546875" style="6" customWidth="1"/>
+    <col min="11" max="11" width="25" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="16" t="s">
         <v>99</v>
       </c>
       <c r="B1" s="16" t="s">
+        <v>386</v>
+      </c>
+      <c r="C1" s="16" t="s">
+        <v>383</v>
+      </c>
+      <c r="D1" s="16" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="2" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
+        <v>298</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>394</v>
+      </c>
+      <c r="C2" s="9"/>
+      <c r="D2" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="E2" s="5"/>
+    </row>
+    <row r="3" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>394</v>
+      </c>
+      <c r="C3" s="3"/>
+      <c r="D3" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="E3" s="5"/>
+    </row>
+    <row r="4" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>394</v>
+      </c>
+      <c r="C4" s="3"/>
+      <c r="D4" s="2" t="s">
+        <v>250</v>
+      </c>
+      <c r="F4" s="4"/>
+    </row>
+    <row r="5" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>394</v>
+      </c>
+      <c r="C5" s="3"/>
+      <c r="D5" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="F5" s="4"/>
+    </row>
+    <row r="6" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>394</v>
+      </c>
+      <c r="C6" s="3"/>
+      <c r="D6" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="E6" s="5"/>
+    </row>
+    <row r="7" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>394</v>
+      </c>
+      <c r="C7" s="3"/>
+      <c r="D7" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="E7" s="5"/>
+    </row>
+    <row r="8" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>394</v>
+      </c>
+      <c r="C8" s="3"/>
+      <c r="D8" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="E8" s="5"/>
+    </row>
+    <row r="9" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>394</v>
+      </c>
+      <c r="C9" s="3"/>
+      <c r="D9" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="E9" s="5"/>
+    </row>
+    <row r="10" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>394</v>
+      </c>
+      <c r="C10" s="3"/>
+      <c r="D10" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="E10" s="5"/>
+    </row>
+    <row r="11" spans="1:6" s="5" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>387</v>
+      </c>
+      <c r="C11" s="3"/>
+      <c r="D11" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="F11" s="4"/>
+    </row>
+    <row r="12" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>387</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>396</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>259</v>
+      </c>
+      <c r="E12" s="5"/>
+    </row>
+    <row r="13" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="7" t="s">
+        <v>254</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>387</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>396</v>
+      </c>
+      <c r="D13" s="7" t="s">
+        <v>265</v>
+      </c>
+      <c r="E13" s="5"/>
+    </row>
+    <row r="14" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>387</v>
+      </c>
+      <c r="C14" s="3"/>
+      <c r="D14" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="E14" s="5"/>
+    </row>
+    <row r="15" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="3" t="s">
+        <v>166</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>387</v>
+      </c>
+      <c r="C15" s="3"/>
+      <c r="D15" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="E15" s="24"/>
+    </row>
+    <row r="16" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>387</v>
+      </c>
+      <c r="C16" s="3"/>
+      <c r="D16" s="1" t="s">
+        <v>309</v>
+      </c>
+      <c r="E16" s="24"/>
+    </row>
+    <row r="17" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="9" t="s">
+        <v>107</v>
+      </c>
+      <c r="B17" s="9" t="s">
+        <v>387</v>
+      </c>
+      <c r="C17" s="9"/>
+      <c r="D17" s="3" t="s">
+        <v>153</v>
+      </c>
+      <c r="E17" s="5"/>
+    </row>
+    <row r="18" spans="1:5" s="4" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="18" t="s">
+        <v>247</v>
+      </c>
+      <c r="B18" s="18" t="s">
+        <v>387</v>
+      </c>
+      <c r="C18" s="18"/>
+      <c r="D18" s="18" t="s">
+        <v>246</v>
+      </c>
+      <c r="E18" s="5"/>
+    </row>
+    <row r="19" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="9" t="s">
+        <v>352</v>
+      </c>
+      <c r="B19" s="9" t="s">
+        <v>391</v>
+      </c>
+      <c r="C19" s="9" t="s">
+        <v>392</v>
+      </c>
+      <c r="D19" s="9" t="s">
+        <v>372</v>
+      </c>
+      <c r="E19" s="5"/>
+    </row>
+    <row r="20" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="9" t="s">
+        <v>357</v>
+      </c>
+      <c r="B20" s="9" t="s">
+        <v>391</v>
+      </c>
+      <c r="C20" s="9" t="s">
+        <v>392</v>
+      </c>
+      <c r="D20" s="9" t="s">
+        <v>377</v>
+      </c>
+      <c r="E20" s="5"/>
+    </row>
+    <row r="21" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="9" t="s">
+        <v>354</v>
+      </c>
+      <c r="B21" s="9" t="s">
+        <v>391</v>
+      </c>
+      <c r="C21" s="9" t="s">
+        <v>392</v>
+      </c>
+      <c r="D21" s="9" t="s">
+        <v>374</v>
+      </c>
+      <c r="E21" s="5"/>
+    </row>
+    <row r="22" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="9" t="s">
+        <v>347</v>
+      </c>
+      <c r="B22" s="9" t="s">
+        <v>391</v>
+      </c>
+      <c r="C22" s="9" t="s">
+        <v>392</v>
+      </c>
+      <c r="D22" s="9" t="s">
+        <v>367</v>
+      </c>
+      <c r="E22" s="5"/>
+    </row>
+    <row r="23" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="9" t="s">
+        <v>361</v>
+      </c>
+      <c r="B23" s="9" t="s">
+        <v>391</v>
+      </c>
+      <c r="C23" s="9" t="s">
+        <v>392</v>
+      </c>
+      <c r="D23" s="9" t="s">
+        <v>381</v>
+      </c>
+      <c r="E23" s="5"/>
+    </row>
+    <row r="24" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="9" t="s">
+        <v>356</v>
+      </c>
+      <c r="B24" s="9" t="s">
+        <v>391</v>
+      </c>
+      <c r="C24" s="9" t="s">
+        <v>392</v>
+      </c>
+      <c r="D24" s="9" t="s">
+        <v>376</v>
+      </c>
+      <c r="E24" s="5"/>
+    </row>
+    <row r="25" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="9" t="s">
+        <v>358</v>
+      </c>
+      <c r="B25" s="9" t="s">
+        <v>391</v>
+      </c>
+      <c r="C25" s="9" t="s">
+        <v>392</v>
+      </c>
+      <c r="D25" s="9" t="s">
+        <v>378</v>
+      </c>
+      <c r="E25" s="5"/>
+    </row>
+    <row r="26" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="9" t="s">
+        <v>360</v>
+      </c>
+      <c r="B26" s="9" t="s">
+        <v>391</v>
+      </c>
+      <c r="C26" s="9" t="s">
+        <v>392</v>
+      </c>
+      <c r="D26" s="9" t="s">
+        <v>380</v>
+      </c>
+      <c r="E26" s="5"/>
+    </row>
+    <row r="27" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="9" t="s">
+        <v>349</v>
+      </c>
+      <c r="B27" s="9" t="s">
+        <v>391</v>
+      </c>
+      <c r="C27" s="9" t="s">
+        <v>392</v>
+      </c>
+      <c r="D27" s="9" t="s">
+        <v>369</v>
+      </c>
+      <c r="E27" s="5"/>
+    </row>
+    <row r="28" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="9" t="s">
+        <v>353</v>
+      </c>
+      <c r="B28" s="9" t="s">
+        <v>391</v>
+      </c>
+      <c r="C28" s="9" t="s">
+        <v>392</v>
+      </c>
+      <c r="D28" s="9" t="s">
+        <v>373</v>
+      </c>
+      <c r="E28" s="5"/>
+    </row>
+    <row r="29" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="9" t="s">
+        <v>350</v>
+      </c>
+      <c r="B29" s="9" t="s">
+        <v>391</v>
+      </c>
+      <c r="C29" s="9" t="s">
+        <v>392</v>
+      </c>
+      <c r="D29" s="9" t="s">
+        <v>370</v>
+      </c>
+      <c r="E29" s="24"/>
+    </row>
+    <row r="30" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="9" t="s">
+        <v>348</v>
+      </c>
+      <c r="B30" s="9" t="s">
+        <v>391</v>
+      </c>
+      <c r="C30" s="9" t="s">
+        <v>392</v>
+      </c>
+      <c r="D30" s="9" t="s">
+        <v>368</v>
+      </c>
+      <c r="E30" s="24"/>
+    </row>
+    <row r="31" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="9" t="s">
         <v>291</v>
       </c>
-      <c r="B2" s="9" t="s">
+      <c r="B31" s="9" t="s">
+        <v>397</v>
+      </c>
+      <c r="C31" s="9"/>
+      <c r="D31" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="C2" s="5"/>
-    </row>
-    <row r="3" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="9" t="s">
+      <c r="E31" s="5"/>
+    </row>
+    <row r="32" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="9" t="s">
         <v>295</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B32" s="9" t="s">
+        <v>397</v>
+      </c>
+      <c r="C32" s="9"/>
+      <c r="D32" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="C3" s="5"/>
-    </row>
-    <row r="4" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>241</v>
-      </c>
-      <c r="D4" s="4"/>
-    </row>
-    <row r="5" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="9" t="s">
+      <c r="E32" s="5"/>
+    </row>
+    <row r="33" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="9" t="s">
         <v>285</v>
       </c>
-      <c r="B5" s="9" t="s">
+      <c r="B33" s="9" t="s">
+        <v>397</v>
+      </c>
+      <c r="C33" s="9"/>
+      <c r="D33" s="9" t="s">
         <v>286</v>
       </c>
-      <c r="D5" s="4"/>
-    </row>
-    <row r="6" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>259</v>
-      </c>
-      <c r="C6" s="5"/>
-    </row>
-    <row r="7" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="7" t="s">
-        <v>254</v>
-      </c>
-      <c r="B7" s="7" t="s">
-        <v>265</v>
-      </c>
-      <c r="C7" s="5"/>
-    </row>
-    <row r="8" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="7" t="s">
-        <v>252</v>
-      </c>
-      <c r="B8" s="7" t="s">
-        <v>253</v>
-      </c>
-      <c r="C8" s="5"/>
-    </row>
-    <row r="9" spans="1:4" s="4" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="9" t="s">
+      <c r="E33" s="5"/>
+    </row>
+    <row r="34" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="9" t="s">
         <v>114</v>
       </c>
-      <c r="B9" s="3" t="s">
+      <c r="B34" s="9" t="s">
+        <v>397</v>
+      </c>
+      <c r="C34" s="9"/>
+      <c r="D34" s="3" t="s">
         <v>159</v>
       </c>
-      <c r="C9" s="5"/>
-    </row>
-    <row r="10" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="9" t="s">
+      <c r="E34" s="5"/>
+    </row>
+    <row r="35" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="9" t="s">
         <v>296</v>
       </c>
-      <c r="B10" s="3" t="s">
+      <c r="B35" s="9" t="s">
+        <v>397</v>
+      </c>
+      <c r="C35" s="9"/>
+      <c r="D35" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="C10" s="5"/>
-    </row>
-    <row r="11" spans="1:4" s="5" customFormat="1" ht="14" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="9" t="s">
+      <c r="E35" s="5"/>
+    </row>
+    <row r="36" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="9" t="s">
         <v>297</v>
       </c>
-      <c r="B11" s="3" t="s">
+      <c r="B36" s="9" t="s">
+        <v>397</v>
+      </c>
+      <c r="C36" s="9"/>
+      <c r="D36" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="D11" s="4"/>
-    </row>
-    <row r="12" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="9" t="s">
+      <c r="E36" s="5"/>
+    </row>
+    <row r="37" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="9" t="s">
         <v>105</v>
       </c>
-      <c r="B12" s="3" t="s">
+      <c r="B37" s="9" t="s">
+        <v>397</v>
+      </c>
+      <c r="C37" s="9"/>
+      <c r="D37" s="3" t="s">
         <v>130</v>
       </c>
-      <c r="C12" s="5"/>
-    </row>
-    <row r="13" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="7" t="s">
-        <v>226</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>224</v>
-      </c>
-      <c r="C13" s="5"/>
-    </row>
-    <row r="14" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="3" t="s">
-        <v>106</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>131</v>
-      </c>
-      <c r="C14" s="5"/>
-    </row>
-    <row r="15" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="3" t="s">
+      <c r="E37" s="5"/>
+      <c r="K37" s="10"/>
+      <c r="L37" s="11"/>
+    </row>
+    <row r="38" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="B15" s="1" t="s">
+      <c r="B38" s="9" t="s">
+        <v>397</v>
+      </c>
+      <c r="C38" s="3"/>
+      <c r="D38" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="C15" s="24"/>
-    </row>
-    <row r="16" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="9" t="s">
-        <v>298</v>
-      </c>
-      <c r="B16" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="C16" s="24"/>
-    </row>
-    <row r="17" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="C17" s="5"/>
-    </row>
-    <row r="18" spans="1:3" s="4" customFormat="1" ht="14" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="3" t="s">
+      <c r="E38" s="5"/>
+    </row>
+    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A39" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="B18" s="1" t="s">
+      <c r="B39" s="9" t="s">
+        <v>397</v>
+      </c>
+      <c r="C39" s="3"/>
+      <c r="D39" s="1" t="s">
         <v>242</v>
       </c>
-      <c r="C18" s="5"/>
-    </row>
-    <row r="19" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="7" t="s">
+      <c r="F39" s="4"/>
+    </row>
+    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A40" s="7" t="s">
         <v>255</v>
       </c>
-      <c r="B19" s="7" t="s">
+      <c r="B40" s="9" t="s">
+        <v>397</v>
+      </c>
+      <c r="C40" s="7"/>
+      <c r="D40" s="7" t="s">
         <v>256</v>
       </c>
-      <c r="C19" s="5"/>
-    </row>
-    <row r="20" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="3" t="s">
+      <c r="F40" s="4"/>
+    </row>
+    <row r="41" spans="1:13" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B20" s="2" t="s">
+      <c r="B41" s="9" t="s">
+        <v>397</v>
+      </c>
+      <c r="C41" s="3"/>
+      <c r="D41" s="2" t="s">
         <v>249</v>
       </c>
-      <c r="C20" s="5"/>
-    </row>
-    <row r="21" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B21" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="C21" s="5"/>
-    </row>
-    <row r="22" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="3" t="s">
-        <v>166</v>
-      </c>
-      <c r="B22" s="2" t="s">
-        <v>167</v>
-      </c>
-      <c r="C22" s="5"/>
-    </row>
-    <row r="23" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="B23" s="2" t="s">
-        <v>260</v>
-      </c>
-      <c r="C23" s="5"/>
-    </row>
-    <row r="24" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="B24" s="2" t="s">
-        <v>261</v>
-      </c>
-      <c r="C24" s="5"/>
-    </row>
-    <row r="25" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B25" s="1" t="s">
-        <v>220</v>
-      </c>
-      <c r="C25" s="5"/>
-    </row>
-    <row r="26" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B26" s="2" t="s">
-        <v>221</v>
-      </c>
-      <c r="C26" s="5"/>
-    </row>
-    <row r="27" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B27" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="C27" s="5"/>
-    </row>
-    <row r="28" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="B28" s="1" t="s">
-        <v>309</v>
-      </c>
-      <c r="C28" s="5"/>
-    </row>
-    <row r="29" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B29" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="C29" s="24"/>
-    </row>
-    <row r="30" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="9" t="s">
+      <c r="F41" s="4"/>
+    </row>
+    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A42" s="9" t="s">
         <v>277</v>
       </c>
-      <c r="B30" s="9" t="s">
+      <c r="B42" s="9" t="s">
+        <v>397</v>
+      </c>
+      <c r="C42" s="9"/>
+      <c r="D42" s="9" t="s">
         <v>278</v>
       </c>
-      <c r="C30" s="24"/>
-    </row>
-    <row r="31" spans="1:3" s="4" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="B31" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="C31" s="5"/>
-    </row>
-    <row r="32" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="9" t="s">
+      <c r="F42" s="4"/>
+    </row>
+    <row r="43" spans="1:13" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="9" t="s">
         <v>287</v>
       </c>
-      <c r="B32" s="9" t="s">
+      <c r="B43" s="9" t="s">
+        <v>397</v>
+      </c>
+      <c r="C43" s="9"/>
+      <c r="D43" s="9" t="s">
         <v>288</v>
       </c>
-      <c r="C32" s="5"/>
-    </row>
-    <row r="33" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="9" t="s">
+      <c r="F43" s="4"/>
+    </row>
+    <row r="44" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A44" s="9" t="s">
         <v>289</v>
       </c>
-      <c r="B33" s="9" t="s">
+      <c r="B44" s="9" t="s">
+        <v>397</v>
+      </c>
+      <c r="C44" s="9"/>
+      <c r="D44" s="9" t="s">
         <v>290</v>
       </c>
-      <c r="C33" s="5"/>
-    </row>
-    <row r="34" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="3" t="s">
+      <c r="F44" s="4"/>
+    </row>
+    <row r="45" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A45" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="B34" s="1" t="s">
+      <c r="B45" s="9" t="s">
+        <v>397</v>
+      </c>
+      <c r="C45" s="3"/>
+      <c r="D45" s="1" t="s">
         <v>262</v>
       </c>
-      <c r="C34" s="5"/>
-    </row>
-    <row r="35" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B35" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="C35" s="5"/>
-    </row>
-    <row r="36" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B36" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="C36" s="5"/>
-    </row>
-    <row r="37" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B37" s="1" t="s">
-        <v>248</v>
-      </c>
-      <c r="C37" s="5"/>
-      <c r="I37" s="10"/>
-      <c r="J37" s="11"/>
-    </row>
-    <row r="38" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="3" t="s">
+      <c r="F45" s="4"/>
+    </row>
+    <row r="46" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A46" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="B38" s="2" t="s">
+      <c r="B46" s="9" t="s">
+        <v>397</v>
+      </c>
+      <c r="C46" s="3" t="s">
+        <v>384</v>
+      </c>
+      <c r="D46" s="2" t="s">
         <v>251</v>
       </c>
-      <c r="C38" s="5"/>
-    </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A39" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="B39" s="2" t="s">
-        <v>263</v>
-      </c>
-      <c r="D39" s="4"/>
-    </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A40" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="B40" s="2" t="s">
-        <v>264</v>
-      </c>
-      <c r="D40" s="4"/>
-    </row>
-    <row r="41" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="B41" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="D41" s="4"/>
-    </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A42" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="B42" s="2" t="s">
-        <v>250</v>
-      </c>
-      <c r="D42" s="4"/>
-    </row>
-    <row r="43" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A43" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B43" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="D43" s="4"/>
-    </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A44" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B44" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="D44" s="4"/>
-    </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A45" s="9" t="s">
+      <c r="F46" s="4"/>
+      <c r="K46" s="10"/>
+      <c r="L46" s="11"/>
+      <c r="M46" s="11"/>
+    </row>
+    <row r="47" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A47" s="9" t="s">
         <v>283</v>
       </c>
-      <c r="B45" s="9" t="s">
+      <c r="B47" s="9" t="s">
+        <v>397</v>
+      </c>
+      <c r="C47" s="9"/>
+      <c r="D47" s="9" t="s">
         <v>284</v>
       </c>
-      <c r="D45" s="4"/>
-    </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A46" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B46" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="D46" s="4"/>
-      <c r="I46" s="10"/>
-      <c r="J46" s="11"/>
-      <c r="K46" s="11"/>
-    </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A47" s="9" t="s">
+      <c r="F47" s="4"/>
+      <c r="K47" s="10"/>
+      <c r="L47" s="11"/>
+      <c r="M47" s="11"/>
+    </row>
+    <row r="48" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A48" s="9" t="s">
         <v>299</v>
       </c>
-      <c r="B47" s="3" t="s">
+      <c r="B48" s="9" t="s">
+        <v>397</v>
+      </c>
+      <c r="C48" s="9"/>
+      <c r="D48" s="3" t="s">
         <v>132</v>
       </c>
-      <c r="D47" s="4"/>
-      <c r="I47" s="10"/>
-      <c r="J47" s="11"/>
-      <c r="K47" s="11"/>
-    </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A48" s="9" t="s">
+      <c r="F48" s="4"/>
+      <c r="K48" s="12"/>
+      <c r="L48" s="11"/>
+      <c r="M48" s="11"/>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A49" s="9" t="s">
         <v>124</v>
       </c>
-      <c r="B48" s="3" t="s">
+      <c r="B49" s="9" t="s">
+        <v>397</v>
+      </c>
+      <c r="C49" s="9"/>
+      <c r="D49" s="3" t="s">
         <v>133</v>
       </c>
-      <c r="D48" s="4"/>
-      <c r="I48" s="12"/>
-      <c r="J48" s="11"/>
-      <c r="K48" s="11"/>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A49" s="9" t="s">
+      <c r="F49" s="4"/>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A50" s="9" t="s">
         <v>125</v>
       </c>
-      <c r="B49" s="3" t="s">
+      <c r="B50" s="9" t="s">
+        <v>397</v>
+      </c>
+      <c r="C50" s="9"/>
+      <c r="D50" s="3" t="s">
         <v>134</v>
       </c>
-      <c r="D49" s="4"/>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A50" s="9" t="s">
+      <c r="F50" s="4"/>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A51" s="9" t="s">
         <v>111</v>
       </c>
-      <c r="B50" s="3" t="s">
+      <c r="B51" s="9" t="s">
+        <v>397</v>
+      </c>
+      <c r="C51" s="9"/>
+      <c r="D51" s="3" t="s">
         <v>135</v>
       </c>
-      <c r="D50" s="4"/>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A51" s="9" t="s">
+      <c r="F51" s="4"/>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A52" s="9" t="s">
         <v>300</v>
       </c>
-      <c r="B51" s="3" t="s">
+      <c r="B52" s="9" t="s">
+        <v>397</v>
+      </c>
+      <c r="C52" s="9"/>
+      <c r="D52" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="D51" s="4"/>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A52" s="3" t="s">
+      <c r="F52" s="4"/>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A53" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="B52" s="2" t="s">
+      <c r="B53" s="9" t="s">
+        <v>397</v>
+      </c>
+      <c r="C53" s="3"/>
+      <c r="D53" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="D52" s="4"/>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A53" s="8" t="s">
+      <c r="F53" s="4"/>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A54" s="8" t="s">
         <v>108</v>
       </c>
-      <c r="B53" s="9" t="s">
+      <c r="B54" s="9" t="s">
+        <v>397</v>
+      </c>
+      <c r="C54" s="8"/>
+      <c r="D54" s="9" t="s">
         <v>136</v>
       </c>
-      <c r="D53" s="4"/>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A54" s="3" t="s">
+      <c r="F54" s="4"/>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A55" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="B54" s="2" t="s">
+      <c r="B55" s="9" t="s">
+        <v>397</v>
+      </c>
+      <c r="C55" s="3"/>
+      <c r="D55" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="D54" s="4"/>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A55" s="9" t="s">
+      <c r="F55" s="4"/>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A56" s="9" t="s">
         <v>273</v>
       </c>
-      <c r="B55" s="9" t="s">
+      <c r="B56" s="9" t="s">
+        <v>397</v>
+      </c>
+      <c r="C56" s="9"/>
+      <c r="D56" s="9" t="s">
         <v>274</v>
       </c>
-      <c r="D55" s="4"/>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A56" s="9" t="s">
+      <c r="F56" s="4"/>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A57" s="9" t="s">
         <v>301</v>
       </c>
-      <c r="B56" s="3" t="s">
+      <c r="B57" s="9" t="s">
+        <v>397</v>
+      </c>
+      <c r="C57" s="9"/>
+      <c r="D57" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="D56" s="4"/>
-    </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A57" s="8" t="s">
+      <c r="F57" s="4"/>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A58" s="8" t="s">
         <v>302</v>
       </c>
-      <c r="B57" s="3" t="s">
+      <c r="B58" s="9" t="s">
+        <v>397</v>
+      </c>
+      <c r="C58" s="8"/>
+      <c r="D58" s="3" t="s">
         <v>303</v>
       </c>
-      <c r="D57" s="4"/>
-    </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A58" s="9" t="s">
+      <c r="F58" s="4"/>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A59" s="9" t="s">
         <v>304</v>
       </c>
-      <c r="B58" s="3" t="s">
+      <c r="B59" s="9" t="s">
+        <v>397</v>
+      </c>
+      <c r="C59" s="9"/>
+      <c r="D59" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="D58" s="4"/>
-    </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A59" s="9" t="s">
+      <c r="F59" s="4"/>
+    </row>
+    <row r="60" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A60" s="9" t="s">
         <v>305</v>
       </c>
-      <c r="B59" s="3" t="s">
+      <c r="B60" s="9" t="s">
+        <v>397</v>
+      </c>
+      <c r="C60" s="9"/>
+      <c r="D60" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="D59" s="4"/>
-    </row>
-    <row r="60" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A60" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="B60" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="D60" s="4"/>
-    </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F60" s="4"/>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A61" s="9" t="s">
         <v>104</v>
       </c>
-      <c r="B61" s="3" t="s">
+      <c r="B61" s="9" t="s">
+        <v>397</v>
+      </c>
+      <c r="C61" s="9"/>
+      <c r="D61" s="3" t="s">
         <v>137</v>
       </c>
-      <c r="D61" s="4"/>
-    </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F61" s="4"/>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A62" s="9" t="s">
         <v>116</v>
       </c>
-      <c r="B62" s="3" t="s">
+      <c r="B62" s="9" t="s">
+        <v>397</v>
+      </c>
+      <c r="C62" s="9"/>
+      <c r="D62" s="3" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A63" s="9" t="s">
         <v>123</v>
       </c>
-      <c r="B63" s="3" t="s">
+      <c r="B63" s="9" t="s">
+        <v>397</v>
+      </c>
+      <c r="C63" s="9"/>
+      <c r="D63" s="3" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A64" s="9" t="s">
         <v>117</v>
       </c>
-      <c r="B64" s="3" t="s">
+      <c r="B64" s="9" t="s">
+        <v>397</v>
+      </c>
+      <c r="C64" s="9"/>
+      <c r="D64" s="3" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A65" s="9" t="s">
         <v>115</v>
       </c>
-      <c r="B65" s="3" t="s">
+      <c r="B65" s="9" t="s">
+        <v>397</v>
+      </c>
+      <c r="C65" s="9"/>
+      <c r="D65" s="3" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A66" s="9" t="s">
         <v>122</v>
       </c>
-      <c r="B66" s="3" t="s">
+      <c r="B66" s="9" t="s">
+        <v>397</v>
+      </c>
+      <c r="C66" s="9"/>
+      <c r="D66" s="3" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A67" s="9" t="s">
         <v>127</v>
       </c>
-      <c r="B67" s="3" t="s">
+      <c r="B67" s="9" t="s">
+        <v>397</v>
+      </c>
+      <c r="C67" s="9"/>
+      <c r="D67" s="3" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A68" s="9" t="s">
         <v>102</v>
       </c>
-      <c r="B68" s="3" t="s">
+      <c r="B68" s="9" t="s">
+        <v>397</v>
+      </c>
+      <c r="C68" s="9"/>
+      <c r="D68" s="3" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A69" s="9" t="s">
         <v>126</v>
       </c>
-      <c r="B69" s="3" t="s">
+      <c r="B69" s="9" t="s">
+        <v>397</v>
+      </c>
+      <c r="C69" s="9"/>
+      <c r="D69" s="3" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A70" s="9" t="s">
         <v>109</v>
       </c>
-      <c r="B70" s="3" t="s">
+      <c r="B70" s="9" t="s">
+        <v>397</v>
+      </c>
+      <c r="C70" s="9"/>
+      <c r="D70" s="3" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A71" s="9" t="s">
         <v>121</v>
       </c>
-      <c r="B71" s="3" t="s">
+      <c r="B71" s="9" t="s">
+        <v>397</v>
+      </c>
+      <c r="C71" s="9"/>
+      <c r="D71" s="3" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A72" s="9" t="s">
         <v>120</v>
       </c>
-      <c r="B72" s="3" t="s">
+      <c r="B72" s="9" t="s">
+        <v>397</v>
+      </c>
+      <c r="C72" s="9"/>
+      <c r="D72" s="3" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A73" s="9" t="s">
         <v>119</v>
       </c>
-      <c r="B73" s="3" t="s">
+      <c r="B73" s="9" t="s">
+        <v>397</v>
+      </c>
+      <c r="C73" s="9"/>
+      <c r="D73" s="3" t="s">
         <v>144</v>
       </c>
-      <c r="C73"/>
-      <c r="F73" s="6"/>
-    </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="E73"/>
+      <c r="H73" s="6"/>
+    </row>
+    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A74" s="9" t="s">
         <v>110</v>
       </c>
-      <c r="B74" s="3" t="s">
+      <c r="B74" s="9" t="s">
+        <v>397</v>
+      </c>
+      <c r="C74" s="9"/>
+      <c r="D74" s="3" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A75" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="B75" s="1" t="s">
+      <c r="B75" s="9" t="s">
+        <v>397</v>
+      </c>
+      <c r="C75" s="3"/>
+      <c r="D75" s="1" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A76" s="9" t="s">
         <v>266</v>
       </c>
-      <c r="B76" s="8" t="s">
+      <c r="B76" s="9" t="s">
+        <v>397</v>
+      </c>
+      <c r="C76" s="9"/>
+      <c r="D76" s="8" t="s">
         <v>267</v>
       </c>
     </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A77" s="9" t="s">
+        <v>335</v>
+      </c>
+      <c r="B77" s="9" t="s">
+        <v>397</v>
+      </c>
+      <c r="C77" s="9"/>
+      <c r="D77" s="9" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A78" s="9" t="s">
         <v>269</v>
       </c>
-      <c r="B77" s="9" t="s">
+      <c r="B78" s="9" t="s">
+        <v>397</v>
+      </c>
+      <c r="C78" s="9"/>
+      <c r="D78" s="9" t="s">
         <v>270</v>
       </c>
     </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A78" s="9" t="s">
+    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A79" s="9" t="s">
         <v>271</v>
       </c>
-      <c r="B78" s="9" t="s">
+      <c r="B79" s="9" t="s">
+        <v>397</v>
+      </c>
+      <c r="C79" s="9"/>
+      <c r="D79" s="9" t="s">
         <v>272</v>
       </c>
     </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A79" s="9" t="s">
-        <v>335</v>
-      </c>
-      <c r="B79" s="9" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A80" s="9" t="s">
         <v>279</v>
       </c>
       <c r="B80" s="9" t="s">
+        <v>397</v>
+      </c>
+      <c r="C80" s="9"/>
+      <c r="D80" s="9" t="s">
         <v>280</v>
       </c>
     </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A81" s="9" t="s">
         <v>281</v>
       </c>
       <c r="B81" s="9" t="s">
+        <v>397</v>
+      </c>
+      <c r="C81" s="9"/>
+      <c r="D81" s="9" t="s">
         <v>282</v>
       </c>
     </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A82" s="3" t="s">
+    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A82" s="9" t="s">
+        <v>118</v>
+      </c>
+      <c r="B82" s="9" t="s">
+        <v>397</v>
+      </c>
+      <c r="C82" s="9"/>
+      <c r="D82" s="3" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A83" s="9" t="s">
+        <v>306</v>
+      </c>
+      <c r="B83" s="9" t="s">
+        <v>397</v>
+      </c>
+      <c r="C83" s="9"/>
+      <c r="D83" s="3" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A84" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B84" s="9" t="s">
+        <v>397</v>
+      </c>
+      <c r="C84" s="3"/>
+      <c r="D84" s="1" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A85" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="B85" s="9" t="s">
+        <v>397</v>
+      </c>
+      <c r="C85" s="9"/>
+      <c r="D85" s="3" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A86" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B86" s="9" t="s">
+        <v>397</v>
+      </c>
+      <c r="C86" s="3"/>
+      <c r="D86" s="1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A87" s="18" t="s">
+        <v>310</v>
+      </c>
+      <c r="B87" s="9" t="s">
+        <v>397</v>
+      </c>
+      <c r="C87" s="18"/>
+      <c r="D87" s="18" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A88" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B88" s="9" t="s">
+        <v>397</v>
+      </c>
+      <c r="C88" s="3"/>
+      <c r="D88" s="1" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A89" s="9" t="s">
+        <v>128</v>
+      </c>
+      <c r="B89" s="9" t="s">
+        <v>397</v>
+      </c>
+      <c r="C89" s="9"/>
+      <c r="D89" s="9" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A90" s="9" t="s">
+        <v>113</v>
+      </c>
+      <c r="B90" s="9" t="s">
+        <v>397</v>
+      </c>
+      <c r="C90" s="9"/>
+      <c r="D90" s="9" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A91" s="9" t="s">
+        <v>112</v>
+      </c>
+      <c r="B91" s="9" t="s">
+        <v>397</v>
+      </c>
+      <c r="C91" s="9"/>
+      <c r="D91" s="3" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A92" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B92" s="9" t="s">
+        <v>397</v>
+      </c>
+      <c r="C92" s="3"/>
+      <c r="D92" s="1" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A93" s="9" t="s">
+        <v>307</v>
+      </c>
+      <c r="B93" s="9" t="s">
+        <v>397</v>
+      </c>
+      <c r="C93" s="9"/>
+      <c r="D93" s="3" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A94" s="9" t="s">
+        <v>275</v>
+      </c>
+      <c r="B94" s="9" t="s">
+        <v>397</v>
+      </c>
+      <c r="C94" s="9"/>
+      <c r="D94" s="9" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A95" s="9" t="s">
+        <v>308</v>
+      </c>
+      <c r="B95" s="9" t="s">
+        <v>397</v>
+      </c>
+      <c r="C95" s="9"/>
+      <c r="D95" s="3" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A96" s="9" t="s">
+        <v>293</v>
+      </c>
+      <c r="B96" s="9" t="s">
+        <v>397</v>
+      </c>
+      <c r="C96" s="9"/>
+      <c r="D96" s="9" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A97" s="9" t="s">
+        <v>100</v>
+      </c>
+      <c r="B97" s="9" t="s">
+        <v>397</v>
+      </c>
+      <c r="C97" s="9"/>
+      <c r="D97" s="3" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A98" s="9" t="s">
+        <v>217</v>
+      </c>
+      <c r="B98" s="9" t="s">
+        <v>397</v>
+      </c>
+      <c r="C98" s="9"/>
+      <c r="D98" s="9" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A99" s="7" t="s">
+        <v>252</v>
+      </c>
+      <c r="B99" s="7" t="s">
+        <v>388</v>
+      </c>
+      <c r="C99" s="7"/>
+      <c r="D99" s="7" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A100" s="9" t="s">
+        <v>351</v>
+      </c>
+      <c r="B100" s="9" t="s">
+        <v>391</v>
+      </c>
+      <c r="C100" s="9"/>
+      <c r="D100" s="9" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A101" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B101" s="3" t="s">
+        <v>388</v>
+      </c>
+      <c r="C101" s="3"/>
+      <c r="D101" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A102" s="9" t="s">
+        <v>362</v>
+      </c>
+      <c r="B102" s="9" t="s">
+        <v>388</v>
+      </c>
+      <c r="C102" s="9"/>
+      <c r="D102" s="9" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A103" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B103" s="3" t="s">
+        <v>388</v>
+      </c>
+      <c r="C103" s="3"/>
+      <c r="D103" s="1" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A104" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B104" s="3" t="s">
+        <v>388</v>
+      </c>
+      <c r="C104" s="3"/>
+      <c r="D104" s="2" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A105" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B105" s="3" t="s">
+        <v>388</v>
+      </c>
+      <c r="C105" s="3"/>
+      <c r="D105" s="1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A106" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B106" s="3" t="s">
+        <v>388</v>
+      </c>
+      <c r="C106" s="3"/>
+      <c r="D106" s="1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A107" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B107" s="3" t="s">
+        <v>388</v>
+      </c>
+      <c r="C107" s="3"/>
+      <c r="D107" s="1" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A108" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B108" s="3" t="s">
+        <v>388</v>
+      </c>
+      <c r="C108" s="3" t="s">
+        <v>385</v>
+      </c>
+      <c r="D108" s="1" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A109" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B109" s="3" t="s">
+        <v>388</v>
+      </c>
+      <c r="C109" s="3"/>
+      <c r="D109" s="1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A110" s="9" t="s">
+        <v>359</v>
+      </c>
+      <c r="B110" s="9" t="s">
+        <v>391</v>
+      </c>
+      <c r="C110" s="9"/>
+      <c r="D110" s="9" t="s">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A111" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="B82" s="1" t="s">
+      <c r="B111" s="3" t="s">
+        <v>388</v>
+      </c>
+      <c r="C111" s="3"/>
+      <c r="D111" s="1" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A83" s="3" t="s">
+    <row r="112" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A112" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="B83" s="1" t="s">
+      <c r="B112" s="3" t="s">
+        <v>388</v>
+      </c>
+      <c r="C112" s="3"/>
+      <c r="D112" s="1" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A84" s="9" t="s">
-        <v>118</v>
-      </c>
-      <c r="B84" s="3" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A85" s="9" t="s">
-        <v>306</v>
-      </c>
-      <c r="B85" s="3" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="86" spans="1:2" ht="30" x14ac:dyDescent="0.2">
-      <c r="A86" s="3" t="s">
+    <row r="113" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A113" s="9" t="s">
+        <v>355</v>
+      </c>
+      <c r="B113" s="9" t="s">
+        <v>391</v>
+      </c>
+      <c r="C113" s="9"/>
+      <c r="D113" s="9" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="114" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A114" s="3" t="s">
         <v>129</v>
       </c>
-      <c r="B86" s="1" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A87" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="B87" s="1" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A88" s="9" t="s">
-        <v>103</v>
-      </c>
-      <c r="B88" s="3" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A89" s="3" t="s">
+      <c r="B114" s="3" t="s">
+        <v>388</v>
+      </c>
+      <c r="C114" s="3"/>
+      <c r="D114" s="1" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="115" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A115" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="B89" s="1" t="s">
+      <c r="B115" s="3" t="s">
+        <v>388</v>
+      </c>
+      <c r="C115" s="3"/>
+      <c r="D115" s="1" t="s">
         <v>237</v>
       </c>
     </row>
-    <row r="90" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A90" s="3" t="s">
+    <row r="116" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A116" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B90" s="2" t="s">
+      <c r="B116" s="3" t="s">
+        <v>388</v>
+      </c>
+      <c r="C116" s="3"/>
+      <c r="D116" s="2" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A91" s="7" t="s">
+    <row r="117" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A117" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B117" s="3" t="s">
+        <v>388</v>
+      </c>
+      <c r="C117" s="3"/>
+      <c r="D117" s="1" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="118" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A118" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B118" s="3" t="s">
+        <v>388</v>
+      </c>
+      <c r="C118" s="3"/>
+      <c r="D118" s="1" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="119" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A119" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B119" s="3" t="s">
+        <v>388</v>
+      </c>
+      <c r="C119" s="3"/>
+      <c r="D119" s="2" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="120" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A120" s="7" t="s">
+        <v>294</v>
+      </c>
+      <c r="B120" s="7" t="s">
+        <v>388</v>
+      </c>
+      <c r="C120" s="7"/>
+      <c r="D120" s="2" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="121" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A121" s="7" t="s">
+        <v>257</v>
+      </c>
+      <c r="B121" s="7" t="s">
+        <v>388</v>
+      </c>
+      <c r="C121" s="7"/>
+      <c r="D121" s="7" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="122" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A122" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B122" s="3" t="s">
+        <v>389</v>
+      </c>
+      <c r="C122" s="3"/>
+      <c r="D122" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="123" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A123" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B123" s="3" t="s">
+        <v>389</v>
+      </c>
+      <c r="C123" s="3"/>
+      <c r="D123" s="1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="124" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A124" s="7" t="s">
+        <v>226</v>
+      </c>
+      <c r="B124" s="7" t="s">
+        <v>393</v>
+      </c>
+      <c r="C124" s="7"/>
+      <c r="D124" s="2" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="125" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A125" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="B125" s="7" t="s">
+        <v>393</v>
+      </c>
+      <c r="C125" s="3"/>
+      <c r="D125" s="2" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="126" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A126" s="9" t="s">
+        <v>345</v>
+      </c>
+      <c r="B126" s="9" t="s">
+        <v>393</v>
+      </c>
+      <c r="C126" s="9"/>
+      <c r="D126" s="9" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="127" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A127" s="9" t="s">
+        <v>346</v>
+      </c>
+      <c r="B127" s="9" t="s">
+        <v>393</v>
+      </c>
+      <c r="C127" s="9"/>
+      <c r="D127" s="9" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="128" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A128" s="7" t="s">
         <v>225</v>
       </c>
-      <c r="B91" s="2" t="s">
+      <c r="B128" s="7" t="s">
+        <v>393</v>
+      </c>
+      <c r="C128" s="7"/>
+      <c r="D128" s="2" t="s">
         <v>223</v>
       </c>
     </row>
-    <row r="92" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A92" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="B92" s="1" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="93" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A93" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="B93" s="1" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="94" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A94" s="3" t="s">
+    <row r="129" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A129" s="9" t="s">
+        <v>364</v>
+      </c>
+      <c r="B129" s="9" t="s">
+        <v>393</v>
+      </c>
+      <c r="C129" s="9"/>
+      <c r="D129" s="9" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="130" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A130" s="9" t="s">
+        <v>340</v>
+      </c>
+      <c r="B130" s="9" t="s">
+        <v>393</v>
+      </c>
+      <c r="C130" s="9"/>
+      <c r="D130" s="9" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="131" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A131" s="9" t="s">
+        <v>365</v>
+      </c>
+      <c r="B131" s="9" t="s">
+        <v>393</v>
+      </c>
+      <c r="C131" s="9"/>
+      <c r="D131" s="9" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="132" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A132" s="9" t="s">
+        <v>363</v>
+      </c>
+      <c r="B132" s="9" t="s">
+        <v>393</v>
+      </c>
+      <c r="C132" s="9"/>
+      <c r="D132" s="9" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="133" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A133" s="9" t="s">
+        <v>366</v>
+      </c>
+      <c r="B133" s="9" t="s">
+        <v>393</v>
+      </c>
+      <c r="C133" s="9"/>
+      <c r="D133" s="9" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="134" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A134" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="B134" s="7" t="s">
+        <v>398</v>
+      </c>
+      <c r="C134" s="7"/>
+      <c r="D134" s="2" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="135" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A135" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="B135" s="7" t="s">
+        <v>398</v>
+      </c>
+      <c r="C135" s="7"/>
+      <c r="D135" s="2" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="136" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A136" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B136" s="7" t="s">
+        <v>398</v>
+      </c>
+      <c r="C136" s="3"/>
+      <c r="D136" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="137" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A137" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="B137" s="7" t="s">
+        <v>398</v>
+      </c>
+      <c r="C137" s="7"/>
+      <c r="D137" s="2" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="138" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A138" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="B138" s="7" t="s">
+        <v>398</v>
+      </c>
+      <c r="C138" s="7"/>
+      <c r="D138" s="2" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="139" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A139" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B94" s="1" t="s">
+      <c r="B139" s="3" t="s">
+        <v>398</v>
+      </c>
+      <c r="C139" s="3"/>
+      <c r="D139" s="1" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="95" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A95" s="9" t="s">
-        <v>107</v>
-      </c>
-      <c r="B95" s="3" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="96" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A96" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B96" s="1" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A97" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="B97" s="1" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="98" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A98" s="9" t="s">
-        <v>128</v>
-      </c>
-      <c r="B98" s="9" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="99" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A99" s="9" t="s">
-        <v>113</v>
-      </c>
-      <c r="B99" s="9" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="100" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A100" s="9" t="s">
-        <v>112</v>
-      </c>
-      <c r="B100" s="3" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="101" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A101" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="B101" s="1" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="102" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A102" s="9" t="s">
-        <v>307</v>
-      </c>
-      <c r="B102" s="3" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="103" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A103" s="9" t="s">
-        <v>275</v>
-      </c>
-      <c r="B103" s="9" t="s">
-        <v>276</v>
-      </c>
-    </row>
-    <row r="104" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A104" s="9" t="s">
-        <v>308</v>
-      </c>
-      <c r="B104" s="3" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="105" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A105" s="9" t="s">
-        <v>293</v>
-      </c>
-      <c r="B105" s="9" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="106" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A106" s="9" t="s">
-        <v>100</v>
-      </c>
-      <c r="B106" s="3" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="107" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A107" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="B107" s="1" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="108" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A108" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="B108" s="1" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="109" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A109" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="B109" s="2" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="110" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A110" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="B110" s="2" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="111" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A111" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="B111" s="2" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="112" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A112" s="9" t="s">
-        <v>217</v>
-      </c>
-      <c r="B112" s="9" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="113" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A113" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="B113" s="2" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="114" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A114" s="7" t="s">
-        <v>294</v>
-      </c>
-      <c r="B114" s="2" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="115" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A115" s="7" t="s">
-        <v>257</v>
-      </c>
-      <c r="B115" s="7" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="116" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A116" s="18" t="s">
-        <v>247</v>
-      </c>
-      <c r="B116" s="18" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="117" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A117" s="18" t="s">
-        <v>310</v>
-      </c>
-      <c r="B117" s="18" t="s">
-        <v>311</v>
-      </c>
-    </row>
-    <row r="118" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A118" s="18" t="s">
+    <row r="140" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A140" s="18" t="s">
+        <v>329</v>
+      </c>
+      <c r="B140" s="18" t="s">
+        <v>400</v>
+      </c>
+      <c r="C140" s="18" t="s">
+        <v>399</v>
+      </c>
+      <c r="D140" s="18" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="141" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A141" s="18" t="s">
+        <v>331</v>
+      </c>
+      <c r="B141" s="18" t="s">
+        <v>400</v>
+      </c>
+      <c r="C141" s="18" t="s">
+        <v>399</v>
+      </c>
+      <c r="D141" s="18" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="142" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A142" s="18" t="s">
+        <v>316</v>
+      </c>
+      <c r="B142" s="18" t="s">
+        <v>400</v>
+      </c>
+      <c r="C142" s="18" t="s">
+        <v>399</v>
+      </c>
+      <c r="D142" s="18" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="143" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A143" s="18" t="s">
+        <v>314</v>
+      </c>
+      <c r="B143" s="18" t="s">
+        <v>400</v>
+      </c>
+      <c r="C143" s="18" t="s">
+        <v>399</v>
+      </c>
+      <c r="D143" s="18" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="144" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A144" s="18" t="s">
         <v>312</v>
       </c>
-      <c r="B118" s="18" t="s">
+      <c r="B144" s="18" t="s">
+        <v>400</v>
+      </c>
+      <c r="C144" s="18" t="s">
+        <v>399</v>
+      </c>
+      <c r="D144" s="18" t="s">
         <v>313</v>
       </c>
     </row>
-    <row r="119" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A119" s="18" t="s">
-        <v>314</v>
-      </c>
-      <c r="B119" s="18" t="s">
-        <v>315</v>
-      </c>
-    </row>
-    <row r="120" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A120" s="18" t="s">
-        <v>316</v>
-      </c>
-      <c r="B120" s="18" t="s">
-        <v>317</v>
-      </c>
-    </row>
-    <row r="121" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A121" s="18" t="s">
+    <row r="145" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A145" s="18" t="s">
         <v>318</v>
       </c>
-      <c r="B121" s="18" t="s">
+      <c r="B145" s="18" t="s">
+        <v>400</v>
+      </c>
+      <c r="C145" s="18" t="s">
+        <v>399</v>
+      </c>
+      <c r="D145" s="18" t="s">
         <v>319</v>
       </c>
     </row>
-    <row r="122" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A122" s="18" t="s">
+    <row r="146" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A146" s="18" t="s">
         <v>320</v>
       </c>
-      <c r="B122" s="18" t="s">
+      <c r="B146" s="18" t="s">
+        <v>400</v>
+      </c>
+      <c r="C146" s="18" t="s">
+        <v>399</v>
+      </c>
+      <c r="D146" s="18" t="s">
         <v>321</v>
       </c>
     </row>
-    <row r="123" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A123" s="18" t="s">
+    <row r="147" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A147" s="18" t="s">
+        <v>333</v>
+      </c>
+      <c r="B147" s="18" t="s">
+        <v>400</v>
+      </c>
+      <c r="C147" s="18" t="s">
+        <v>399</v>
+      </c>
+      <c r="D147" s="18" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="148" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A148" s="18" t="s">
+        <v>327</v>
+      </c>
+      <c r="B148" s="18" t="s">
+        <v>400</v>
+      </c>
+      <c r="C148" s="18" t="s">
+        <v>399</v>
+      </c>
+      <c r="D148" s="18" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="149" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A149" s="18" t="s">
         <v>322</v>
       </c>
-      <c r="B123" s="18" t="s">
+      <c r="B149" s="18" t="s">
+        <v>400</v>
+      </c>
+      <c r="C149" s="18" t="s">
+        <v>399</v>
+      </c>
+      <c r="D149" s="18" t="s">
         <v>323</v>
       </c>
     </row>
-    <row r="124" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A124" s="18" t="s">
+    <row r="150" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A150" s="18" t="s">
+        <v>336</v>
+      </c>
+      <c r="B150" s="18" t="s">
+        <v>400</v>
+      </c>
+      <c r="C150" s="18" t="s">
+        <v>399</v>
+      </c>
+      <c r="D150" s="18" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="151" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A151" s="18" t="s">
         <v>324</v>
       </c>
-      <c r="B124" s="18" t="s">
+      <c r="B151" s="18" t="s">
+        <v>400</v>
+      </c>
+      <c r="C151" s="18" t="s">
+        <v>399</v>
+      </c>
+      <c r="D151" s="18" t="s">
         <v>325</v>
       </c>
     </row>
-    <row r="125" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A125" s="18" t="s">
-        <v>336</v>
-      </c>
-      <c r="B125" s="18" t="s">
-        <v>326</v>
-      </c>
-    </row>
-    <row r="126" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A126" s="18" t="s">
-        <v>327</v>
-      </c>
-      <c r="B126" s="18" t="s">
-        <v>328</v>
-      </c>
-    </row>
-    <row r="127" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A127" s="18" t="s">
-        <v>329</v>
-      </c>
-      <c r="B127" s="18" t="s">
-        <v>330</v>
-      </c>
-    </row>
-    <row r="128" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A128" s="18" t="s">
-        <v>331</v>
-      </c>
-      <c r="B128" s="18" t="s">
-        <v>332</v>
-      </c>
-    </row>
-    <row r="129" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A129" s="18" t="s">
-        <v>333</v>
-      </c>
-      <c r="B129" s="18" t="s">
-        <v>334</v>
-      </c>
-    </row>
-    <row r="130" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A130" s="9" t="s">
-        <v>347</v>
-      </c>
-      <c r="B130" s="9" t="s">
-        <v>367</v>
-      </c>
-    </row>
-    <row r="131" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A131" s="9" t="s">
-        <v>348</v>
-      </c>
-      <c r="B131" s="9" t="s">
-        <v>368</v>
-      </c>
-    </row>
-    <row r="132" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A132" s="9" t="s">
-        <v>349</v>
-      </c>
-      <c r="B132" s="9" t="s">
-        <v>369</v>
-      </c>
-    </row>
-    <row r="133" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A133" s="9" t="s">
-        <v>350</v>
-      </c>
-      <c r="B133" s="9" t="s">
-        <v>370</v>
-      </c>
-    </row>
-    <row r="134" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A134" s="9" t="s">
-        <v>351</v>
-      </c>
-      <c r="B134" s="9" t="s">
-        <v>371</v>
-      </c>
-    </row>
-    <row r="135" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A135" s="9" t="s">
-        <v>352</v>
-      </c>
-      <c r="B135" s="9" t="s">
-        <v>372</v>
-      </c>
-    </row>
-    <row r="136" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A136" s="9" t="s">
-        <v>353</v>
-      </c>
-      <c r="B136" s="9" t="s">
-        <v>373</v>
-      </c>
-    </row>
-    <row r="137" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A137" s="9" t="s">
-        <v>354</v>
-      </c>
-      <c r="B137" s="9" t="s">
-        <v>374</v>
-      </c>
-    </row>
-    <row r="138" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A138" s="9" t="s">
-        <v>355</v>
-      </c>
-      <c r="B138" s="9" t="s">
-        <v>375</v>
-      </c>
-    </row>
-    <row r="139" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A139" s="9" t="s">
-        <v>356</v>
-      </c>
-      <c r="B139" s="9" t="s">
-        <v>376</v>
-      </c>
-    </row>
-    <row r="140" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A140" s="9" t="s">
-        <v>357</v>
-      </c>
-      <c r="B140" s="9" t="s">
-        <v>377</v>
-      </c>
-    </row>
-    <row r="141" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A141" s="9" t="s">
-        <v>358</v>
-      </c>
-      <c r="B141" s="9" t="s">
-        <v>378</v>
-      </c>
-    </row>
-    <row r="142" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A142" s="9" t="s">
-        <v>359</v>
-      </c>
-      <c r="B142" s="9" t="s">
-        <v>379</v>
-      </c>
-    </row>
-    <row r="143" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A143" s="9" t="s">
-        <v>360</v>
-      </c>
-      <c r="B143" s="9" t="s">
-        <v>380</v>
-      </c>
-    </row>
-    <row r="144" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A144" s="9" t="s">
-        <v>361</v>
-      </c>
-      <c r="B144" s="9" t="s">
-        <v>381</v>
-      </c>
-    </row>
-    <row r="145" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A145" s="9" t="s">
-        <v>362</v>
-      </c>
-      <c r="B145" s="9" t="s">
-        <v>382</v>
-      </c>
-    </row>
-    <row r="146" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A146" s="9" t="s">
-        <v>345</v>
-      </c>
-      <c r="B146" s="9" t="s">
-        <v>337</v>
-      </c>
-    </row>
-    <row r="147" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A147" s="9" t="s">
-        <v>346</v>
-      </c>
-      <c r="B147" s="9" t="s">
-        <v>338</v>
-      </c>
-    </row>
-    <row r="148" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A148" s="9" t="s">
-        <v>363</v>
-      </c>
-      <c r="B148" s="9" t="s">
-        <v>339</v>
-      </c>
-    </row>
-    <row r="149" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A149" s="9" t="s">
-        <v>340</v>
-      </c>
-      <c r="B149" s="9" t="s">
-        <v>341</v>
-      </c>
-    </row>
-    <row r="150" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A150" s="9" t="s">
-        <v>364</v>
-      </c>
-      <c r="B150" s="9" t="s">
-        <v>342</v>
-      </c>
-    </row>
-    <row r="151" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A151" s="9" t="s">
-        <v>365</v>
-      </c>
-      <c r="B151" s="9" t="s">
-        <v>343</v>
-      </c>
-    </row>
-    <row r="152" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A152" s="9" t="s">
-        <v>366</v>
-      </c>
-      <c r="B152" s="9" t="s">
-        <v>344</v>
-      </c>
-    </row>
-    <row r="154" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B154" s="13" t="s">
+    <row r="152" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A152" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B152" s="7" t="s">
+        <v>395</v>
+      </c>
+      <c r="C152" s="3"/>
+      <c r="D152" s="2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="154" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D154" s="13" t="s">
         <v>168</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:B129"/>
-  <sortState ref="A2:B101">
+  <autoFilter ref="A1:D152" xr:uid="{00000000-0009-0000-0000-000000000000}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D152">
+      <sortCondition ref="B1:B152"/>
+    </sortState>
+  </autoFilter>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D101">
     <sortCondition ref="A2:A101"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup scale="64" orientation="portrait" verticalDpi="0"/>
+  <pageSetup scale="64" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F123"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B121" sqref="B121"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="28" customWidth="1"/>
-    <col min="2" max="2" width="235.5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="235.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="235.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="235.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="15" t="s">
         <v>219</v>
       </c>
@@ -3597,7 +4324,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
         <v>183</v>
       </c>
@@ -3608,7 +4335,7 @@
       <c r="E2" s="6"/>
       <c r="F2" s="6"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
         <v>191</v>
       </c>
@@ -3619,7 +4346,7 @@
       <c r="E3" s="6"/>
       <c r="F3" s="6"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
         <v>192</v>
       </c>
@@ -3630,7 +4357,7 @@
       <c r="E4" s="6"/>
       <c r="F4" s="6"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="9" t="s">
         <v>190</v>
       </c>
@@ -3641,7 +4368,7 @@
       <c r="E5" s="6"/>
       <c r="F5" s="6"/>
     </row>
-    <row r="6" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="9" t="s">
         <v>285</v>
       </c>
@@ -3649,7 +4376,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
         <v>254</v>
       </c>
@@ -3659,7 +4386,7 @@
       <c r="E7" s="6"/>
       <c r="F7" s="6"/>
     </row>
-    <row r="8" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="9" t="s">
         <v>180</v>
       </c>
@@ -3668,7 +4395,7 @@
       </c>
       <c r="D8"/>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
         <v>252</v>
       </c>
@@ -3678,7 +4405,7 @@
       <c r="E9" s="6"/>
       <c r="F9" s="6"/>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="9" t="s">
         <v>114</v>
       </c>
@@ -3689,7 +4416,7 @@
       <c r="E10" s="6"/>
       <c r="F10" s="6"/>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="9" t="s">
         <v>193</v>
       </c>
@@ -3700,7 +4427,7 @@
       <c r="E11" s="6"/>
       <c r="F11" s="6"/>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="9" t="s">
         <v>195</v>
       </c>
@@ -3710,7 +4437,7 @@
       <c r="E12" s="6"/>
       <c r="F12" s="6"/>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="9" t="s">
         <v>105</v>
       </c>
@@ -3720,7 +4447,7 @@
       <c r="E13" s="6"/>
       <c r="F13" s="6"/>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="9" t="s">
         <v>106</v>
       </c>
@@ -3731,7 +4458,7 @@
       <c r="E14" s="6"/>
       <c r="F14" s="6"/>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="9" t="s">
         <v>187</v>
       </c>
@@ -3742,7 +4469,7 @@
       <c r="E15" s="6"/>
       <c r="F15" s="6"/>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="9" t="s">
         <v>196</v>
       </c>
@@ -3753,7 +4480,7 @@
       <c r="E16" s="6"/>
       <c r="F16" s="6"/>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="9" t="s">
         <v>197</v>
       </c>
@@ -3764,7 +4491,7 @@
       <c r="E17" s="6"/>
       <c r="F17" s="6"/>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="9" t="s">
         <v>17</v>
       </c>
@@ -3775,7 +4502,7 @@
       <c r="E18" s="6"/>
       <c r="F18" s="6"/>
     </row>
-    <row r="19" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="9" t="s">
         <v>21</v>
       </c>
@@ -3784,7 +4511,7 @@
       </c>
       <c r="D19"/>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="7" t="s">
         <v>255</v>
       </c>
@@ -3795,7 +4522,7 @@
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="9" t="s">
         <v>198</v>
       </c>
@@ -3805,7 +4532,7 @@
       <c r="E21" s="6"/>
       <c r="F21" s="6"/>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
         <v>239</v>
       </c>
@@ -3816,7 +4543,7 @@
       <c r="E22" s="6"/>
       <c r="F22" s="6"/>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="9" t="s">
         <v>166</v>
       </c>
@@ -3827,7 +4554,7 @@
       <c r="E23" s="6"/>
       <c r="F23" s="6"/>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="9" t="s">
         <v>177</v>
       </c>
@@ -3838,7 +4565,7 @@
       <c r="E24" s="6"/>
       <c r="F24" s="6"/>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="9" t="s">
         <v>185</v>
       </c>
@@ -3849,7 +4576,7 @@
       <c r="E25" s="6"/>
       <c r="F25" s="6"/>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="9" t="s">
         <v>173</v>
       </c>
@@ -3860,7 +4587,7 @@
       <c r="E26" s="6"/>
       <c r="F26" s="6"/>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="9" t="s">
         <v>200</v>
       </c>
@@ -3871,7 +4598,7 @@
       <c r="E27" s="6"/>
       <c r="F27" s="6"/>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="9" t="s">
         <v>199</v>
       </c>
@@ -3882,7 +4609,7 @@
       <c r="E28" s="6"/>
       <c r="F28" s="6"/>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="9" t="s">
         <v>171</v>
       </c>
@@ -3893,7 +4620,7 @@
       <c r="E29" s="6"/>
       <c r="F29" s="6"/>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" s="9" t="s">
         <v>8</v>
       </c>
@@ -3904,7 +4631,7 @@
       <c r="E30" s="6"/>
       <c r="F30" s="6"/>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" s="9" t="s">
         <v>179</v>
       </c>
@@ -3915,7 +4642,7 @@
       <c r="E31" s="6"/>
       <c r="F31" s="6"/>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" s="9" t="s">
         <v>0</v>
       </c>
@@ -3925,7 +4652,7 @@
       <c r="E32" s="6"/>
       <c r="F32" s="6"/>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" s="9" t="s">
         <v>277</v>
       </c>
@@ -3935,7 +4662,7 @@
       <c r="E33" s="6"/>
       <c r="F33" s="6"/>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" s="9" t="s">
         <v>161</v>
       </c>
@@ -3946,7 +4673,7 @@
       <c r="E34" s="6"/>
       <c r="F34" s="6"/>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" s="9" t="s">
         <v>216</v>
       </c>
@@ -3957,7 +4684,7 @@
       <c r="E35" s="6"/>
       <c r="F35" s="6"/>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" s="9" t="s">
         <v>287</v>
       </c>
@@ -3968,7 +4695,7 @@
       <c r="E36" s="6"/>
       <c r="F36" s="6"/>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" s="9" t="s">
         <v>289</v>
       </c>
@@ -3979,7 +4706,7 @@
       <c r="E37" s="6"/>
       <c r="F37" s="6"/>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" s="9" t="s">
         <v>201</v>
       </c>
@@ -3990,7 +4717,7 @@
       <c r="E38" s="6"/>
       <c r="F38" s="6"/>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" s="9" t="s">
         <v>7</v>
       </c>
@@ -4001,7 +4728,7 @@
       <c r="E39" s="6"/>
       <c r="F39" s="6"/>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" s="9" t="s">
         <v>172</v>
       </c>
@@ -4012,7 +4739,7 @@
       <c r="E40" s="6"/>
       <c r="F40" s="6"/>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" s="9" t="s">
         <v>182</v>
       </c>
@@ -4022,7 +4749,7 @@
       <c r="E41" s="6"/>
       <c r="F41" s="6"/>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" s="9" t="s">
         <v>186</v>
       </c>
@@ -4032,7 +4759,7 @@
       <c r="E42" s="6"/>
       <c r="F42" s="6"/>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" s="9" t="s">
         <v>170</v>
       </c>
@@ -4042,7 +4769,7 @@
       <c r="E43" s="6"/>
       <c r="F43" s="6"/>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" s="9" t="s">
         <v>283</v>
       </c>
@@ -4052,7 +4779,7 @@
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" s="9" t="s">
         <v>169</v>
       </c>
@@ -4062,7 +4789,7 @@
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" s="9" t="s">
         <v>124</v>
       </c>
@@ -4073,7 +4800,7 @@
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" s="9" t="s">
         <v>125</v>
       </c>
@@ -4083,7 +4810,7 @@
       <c r="E47" s="6"/>
       <c r="F47" s="6"/>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" s="9" t="s">
         <v>111</v>
       </c>
@@ -4093,7 +4820,7 @@
       <c r="E48" s="6"/>
       <c r="F48" s="6"/>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" s="9" t="s">
         <v>208</v>
       </c>
@@ -4103,7 +4830,7 @@
       <c r="E49" s="6"/>
       <c r="F49" s="6"/>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" s="9" t="s">
         <v>160</v>
       </c>
@@ -4113,7 +4840,7 @@
       <c r="E50" s="6"/>
       <c r="F50" s="6"/>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51" s="9" t="s">
         <v>108</v>
       </c>
@@ -4123,7 +4850,7 @@
       <c r="E51" s="6"/>
       <c r="F51" s="6"/>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52" s="9" t="s">
         <v>101</v>
       </c>
@@ -4133,7 +4860,7 @@
       <c r="E52" s="6"/>
       <c r="F52" s="6"/>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53" s="9" t="s">
         <v>273</v>
       </c>
@@ -4142,7 +4869,7 @@
       </c>
       <c r="F53" s="6"/>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54" s="9" t="s">
         <v>202</v>
       </c>
@@ -4151,7 +4878,7 @@
       </c>
       <c r="F54" s="6"/>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55" s="9" t="s">
         <v>203</v>
       </c>
@@ -4160,7 +4887,7 @@
       </c>
       <c r="F55" s="6"/>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56" s="9" t="s">
         <v>204</v>
       </c>
@@ -4169,7 +4896,7 @@
       </c>
       <c r="F56" s="6"/>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A57" s="9" t="s">
         <v>207</v>
       </c>
@@ -4178,7 +4905,7 @@
       </c>
       <c r="F57" s="6"/>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A58" s="9" t="s">
         <v>205</v>
       </c>
@@ -4187,7 +4914,7 @@
       </c>
       <c r="F58" s="6"/>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A59" s="9" t="s">
         <v>206</v>
       </c>
@@ -4196,7 +4923,7 @@
       </c>
       <c r="F59" s="6"/>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A60" s="9" t="s">
         <v>104</v>
       </c>
@@ -4205,7 +4932,7 @@
       </c>
       <c r="F60" s="6"/>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A61" s="9" t="s">
         <v>116</v>
       </c>
@@ -4214,7 +4941,7 @@
       </c>
       <c r="F61" s="6"/>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A62" s="9" t="s">
         <v>123</v>
       </c>
@@ -4223,7 +4950,7 @@
       </c>
       <c r="F62" s="6"/>
     </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A63" s="9" t="s">
         <v>117</v>
       </c>
@@ -4232,7 +4959,7 @@
       </c>
       <c r="F63" s="6"/>
     </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A64" s="9" t="s">
         <v>115</v>
       </c>
@@ -4241,7 +4968,7 @@
       </c>
       <c r="F64" s="6"/>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A65" s="9" t="s">
         <v>122</v>
       </c>
@@ -4250,7 +4977,7 @@
       </c>
       <c r="F65" s="6"/>
     </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A66" s="9" t="s">
         <v>127</v>
       </c>
@@ -4259,7 +4986,7 @@
       </c>
       <c r="F66" s="6"/>
     </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A67" s="9" t="s">
         <v>102</v>
       </c>
@@ -4268,7 +4995,7 @@
       </c>
       <c r="F67" s="6"/>
     </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A68" s="9" t="s">
         <v>126</v>
       </c>
@@ -4277,7 +5004,7 @@
       </c>
       <c r="F68" s="6"/>
     </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A69" s="9" t="s">
         <v>109</v>
       </c>
@@ -4286,7 +5013,7 @@
       </c>
       <c r="F69" s="6"/>
     </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A70" s="9" t="s">
         <v>121</v>
       </c>
@@ -4296,7 +5023,7 @@
       <c r="D70" s="6"/>
       <c r="F70" s="6"/>
     </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A71" s="9" t="s">
         <v>120</v>
       </c>
@@ -4305,7 +5032,7 @@
       </c>
       <c r="F71" s="6"/>
     </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A72" s="9" t="s">
         <v>119</v>
       </c>
@@ -4314,7 +5041,7 @@
       </c>
       <c r="F72" s="6"/>
     </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A73" s="9" t="s">
         <v>110</v>
       </c>
@@ -4324,7 +5051,7 @@
       <c r="D73" s="6"/>
       <c r="F73" s="6"/>
     </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A74" s="9" t="s">
         <v>266</v>
       </c>
@@ -4334,7 +5061,7 @@
       <c r="D74" s="6"/>
       <c r="F74" s="6"/>
     </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A75" s="9" t="s">
         <v>269</v>
       </c>
@@ -4344,7 +5071,7 @@
       <c r="D75" s="6"/>
       <c r="F75" s="6"/>
     </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A76" s="9" t="s">
         <v>271</v>
       </c>
@@ -4353,7 +5080,7 @@
       </c>
       <c r="F76" s="6"/>
     </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A77" s="9" t="s">
         <v>335</v>
       </c>
@@ -4362,7 +5089,7 @@
       </c>
       <c r="F77" s="6"/>
     </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A78" s="9" t="s">
         <v>279</v>
       </c>
@@ -4372,7 +5099,7 @@
       <c r="D78" s="6"/>
       <c r="F78" s="6"/>
     </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A79" s="9" t="s">
         <v>281</v>
       </c>
@@ -4382,7 +5109,7 @@
       <c r="D79" s="6"/>
       <c r="F79" s="6"/>
     </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A80" s="9" t="s">
         <v>209</v>
       </c>
@@ -4391,7 +5118,7 @@
       </c>
       <c r="F80" s="6"/>
     </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A81" s="9" t="s">
         <v>118</v>
       </c>
@@ -4401,7 +5128,7 @@
       <c r="D81" s="6"/>
       <c r="F81" s="6"/>
     </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A82" s="9" t="s">
         <v>194</v>
       </c>
@@ -4411,7 +5138,7 @@
       <c r="D82" s="6"/>
       <c r="F82" s="6"/>
     </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A83" s="9" t="s">
         <v>103</v>
       </c>
@@ -4420,7 +5147,7 @@
       </c>
       <c r="F83" s="6"/>
     </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A84" s="9" t="s">
         <v>210</v>
       </c>
@@ -4429,7 +5156,7 @@
       </c>
       <c r="F84" s="6"/>
     </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A85" s="9" t="s">
         <v>18</v>
       </c>
@@ -4438,7 +5165,7 @@
       </c>
       <c r="F85" s="6"/>
     </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A86" s="9" t="s">
         <v>189</v>
       </c>
@@ -4447,7 +5174,7 @@
       </c>
       <c r="F86" s="6"/>
     </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A87" s="9" t="s">
         <v>188</v>
       </c>
@@ -4456,7 +5183,7 @@
       </c>
       <c r="F87" s="6"/>
     </row>
-    <row r="88" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A88" s="9" t="s">
         <v>212</v>
       </c>
@@ -4465,7 +5192,7 @@
       </c>
       <c r="F88" s="6"/>
     </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A89" s="9" t="s">
         <v>213</v>
       </c>
@@ -4474,7 +5201,7 @@
       </c>
       <c r="F89" s="6"/>
     </row>
-    <row r="90" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A90" s="9" t="s">
         <v>174</v>
       </c>
@@ -4483,7 +5210,7 @@
       </c>
       <c r="F90" s="6"/>
     </row>
-    <row r="91" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A91" s="9" t="s">
         <v>176</v>
       </c>
@@ -4493,7 +5220,7 @@
       <c r="D91" s="6"/>
       <c r="F91" s="6"/>
     </row>
-    <row r="92" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A92" s="9" t="s">
         <v>107</v>
       </c>
@@ -4502,7 +5229,7 @@
       </c>
       <c r="D92"/>
     </row>
-    <row r="93" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A93" s="9" t="s">
         <v>5</v>
       </c>
@@ -4512,7 +5239,7 @@
       <c r="D93" s="6"/>
       <c r="F93" s="6"/>
     </row>
-    <row r="94" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A94" s="9" t="s">
         <v>19</v>
       </c>
@@ -4520,7 +5247,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="95" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A95" s="9" t="s">
         <v>128</v>
       </c>
@@ -4528,7 +5255,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="96" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A96" s="9" t="s">
         <v>113</v>
       </c>
@@ -4536,7 +5263,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A97" s="9" t="s">
         <v>112</v>
       </c>
@@ -4544,7 +5271,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="98" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A98" s="9" t="s">
         <v>275</v>
       </c>
@@ -4552,7 +5279,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="99" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A99" s="9" t="s">
         <v>293</v>
       </c>
@@ -4560,7 +5287,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="100" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A100" s="9" t="s">
         <v>100</v>
       </c>
@@ -4568,7 +5295,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="101" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A101" s="9" t="s">
         <v>217</v>
       </c>
@@ -4576,7 +5303,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="102" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A102" s="9" t="s">
         <v>215</v>
       </c>
@@ -4584,7 +5311,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="103" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A103" s="9" t="s">
         <v>211</v>
       </c>
@@ -4592,7 +5319,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="104" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A104" s="9" t="s">
         <v>214</v>
       </c>
@@ -4600,7 +5327,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="105" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A105" s="9" t="s">
         <v>16</v>
       </c>
@@ -4608,7 +5335,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="106" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A106" s="7" t="s">
         <v>257</v>
       </c>
@@ -4616,7 +5343,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="107" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A107" s="22" t="s">
         <v>247</v>
       </c>
@@ -4624,7 +5351,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="108" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A108" s="18" t="s">
         <v>310</v>
       </c>
@@ -4632,7 +5359,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="109" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A109" s="18" t="s">
         <v>312</v>
       </c>
@@ -4640,7 +5367,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="110" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A110" s="18" t="s">
         <v>314</v>
       </c>
@@ -4648,7 +5375,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="111" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A111" s="18" t="s">
         <v>316</v>
       </c>
@@ -4656,7 +5383,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="112" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A112" s="18" t="s">
         <v>318</v>
       </c>
@@ -4664,7 +5391,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="113" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A113" s="18" t="s">
         <v>320</v>
       </c>
@@ -4672,7 +5399,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="114" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A114" s="18" t="s">
         <v>322</v>
       </c>
@@ -4680,7 +5407,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="115" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A115" s="18" t="s">
         <v>324</v>
       </c>
@@ -4688,7 +5415,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="116" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A116" s="18" t="s">
         <v>336</v>
       </c>
@@ -4696,7 +5423,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="117" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A117" s="18" t="s">
         <v>327</v>
       </c>
@@ -4704,7 +5431,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="118" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A118" s="18" t="s">
         <v>329</v>
       </c>
@@ -4712,7 +5439,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="119" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A119" s="18" t="s">
         <v>331</v>
       </c>
@@ -4720,7 +5447,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="120" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A120" s="18" t="s">
         <v>333</v>
       </c>
@@ -4728,7 +5455,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="121" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A121" s="9" t="s">
         <v>362</v>
       </c>
@@ -4736,18 +5463,18 @@
         <v>382</v>
       </c>
     </row>
-    <row r="123" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B123" s="13" t="s">
         <v>168</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:B89">
-    <sortState ref="A2:B107">
+  <autoFilter ref="A1:B121" xr:uid="{00000000-0009-0000-0000-000001000000}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B107">
       <sortCondition ref="A1:A107"/>
     </sortState>
   </autoFilter>
-  <sortState ref="D2:D93">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="D2:D93">
     <sortCondition ref="D53:D144"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4756,20 +5483,20 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:B12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="225.6640625" customWidth="1"/>
+    <col min="1" max="1" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="225.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="17" t="s">
         <v>227</v>
       </c>
@@ -4777,7 +5504,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="18" t="s">
         <v>228</v>
       </c>
@@ -4785,7 +5512,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="18" t="s">
         <v>229</v>
       </c>
@@ -4793,7 +5520,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="18" t="s">
         <v>230</v>
       </c>
@@ -4801,7 +5528,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="18" t="s">
         <v>243</v>
       </c>
@@ -4809,7 +5536,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="18" t="s">
         <v>231</v>
       </c>
@@ -4817,7 +5544,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="18" t="s">
         <v>245</v>
       </c>
@@ -4825,7 +5552,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="18" t="s">
         <v>232</v>
       </c>
@@ -4833,7 +5560,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="18" t="s">
         <v>233</v>
       </c>
@@ -4841,7 +5568,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="30" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="18" t="s">
         <v>234</v>
       </c>
@@ -4849,16 +5576,16 @@
         <v>240</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="20"/>
       <c r="B11" s="20"/>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="20"/>
       <c r="B12" s="21"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:B10"/>
+  <autoFilter ref="A1:B10" xr:uid="{00000000-0009-0000-0000-000002000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0"/>
 </worksheet>

</xml_diff>